<commit_message>
Ajsute turno para pronsotico
Se ajusta para que en la tabla la columna sea el turno y no un consecutivo
</commit_message>
<xml_diff>
--- a/dataset/INFO_MAESTRA_BOM_TIEMPOS.xlsx
+++ b/dataset/INFO_MAESTRA_BOM_TIEMPOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eafit-my.sharepoint.com/personal/wgutierr_eafit_edu_co/Documents/Eafit/V-Logistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eafit-my.sharepoint.com/personal/wgutierr_eafit_edu_co/Documents/Python/Eafit/v-logistics/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{66231F7A-5326-4A92-BE68-FFDEA9C5E602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{675C410D-180E-44D7-8DA7-BBBEBDBF502B}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{66231F7A-5326-4A92-BE68-FFDEA9C5E602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04D3883E-627D-4E08-B136-E4818DDEF274}"/>
   <bookViews>
-    <workbookView xWindow="-30816" yWindow="0" windowWidth="15552" windowHeight="12336" activeTab="3" xr2:uid="{A50434DC-514E-4CB8-92B8-2ABADEF97472}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="3" xr2:uid="{A50434DC-514E-4CB8-92B8-2ABADEF97472}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_MP" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
   <si>
     <t>MOTO</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>COSTO_VBLE_EXTERNO_$xM3</t>
+  </si>
+  <si>
+    <t>PROCESO</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1471,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1499,7 +1502,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1872,11 +1875,12 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="13.921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.15234375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.765625" bestFit="1" customWidth="1"/>

</xml_diff>